<commit_message>
Last day at INTECH
</commit_message>
<xml_diff>
--- a/data/MQTT_tags.xlsx
+++ b/data/MQTT_tags.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\INTECH\Projects\PARCO MFM\lds_comissioning\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5050D534-ED9E-4122-B930-07C3334A7222}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC94B1BB-A704-4248-8896-D469236A4ABE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{FABDB377-5693-4EF3-BB98-FD3465F645EE}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="30">
   <si>
     <t>Periodic</t>
   </si>
@@ -103,6 +103,18 @@
   </si>
   <si>
     <t>NPW_array_PT_5000A</t>
+  </si>
+  <si>
+    <t>PT_62</t>
+  </si>
+  <si>
+    <t>NPW_array_PT_2084</t>
+  </si>
+  <si>
+    <t>NPW_array_PT_4013</t>
+  </si>
+  <si>
+    <t>NPW_array_PT_5013</t>
   </si>
 </sst>
 </file>
@@ -463,10 +475,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26BAE638-D1FF-4458-B2F7-D9A04A7B9A7F}">
-  <dimension ref="A1:L23"/>
+  <dimension ref="A1:L26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -483,13 +495,16 @@
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>26</v>
+      </c>
       <c r="B2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
-        <v>4</v>
+        <v>27</v>
       </c>
       <c r="C3" t="s">
         <v>7</v>
@@ -506,101 +521,116 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="19" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
     </row>
     <row r="20" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="21" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="22" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="23" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="24" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B24" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="25" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B25" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="26" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B26" t="s">
         <v>25</v>
       </c>
     </row>

</xml_diff>